<commit_message>
interface history - Add further missing "Introduced" labels.
</commit_message>
<xml_diff>
--- a/InstallerContent/ASCOMInterfaceRevisions.xlsx
+++ b/InstallerContent/ASCOMInterfaceRevisions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ASCOMPlatform\InstallerContent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6CE6AE-9C36-4CB4-A867-82A42BF31249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D426E2BC-1220-4B98-844D-F6207FC9C8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C77C0BB1-9FCB-4A82-8AED-44FFC5395220}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="315">
   <si>
     <t>Telescope</t>
   </si>
@@ -1224,14 +1224,14 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCFDDAB-B80A-4B5D-BA40-62EFE29ED36B}">
   <dimension ref="A1:F489"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A431" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199:B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,7 +1649,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1" t="s">
         <v>83</v>
       </c>
@@ -1984,7 +1984,9 @@
       <c r="A31" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C31" s="8" t="s">
         <v>308</v>
       </c>
@@ -2335,7 +2337,9 @@
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
+      <c r="E55" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="F55" s="8" t="s">
         <v>308</v>
       </c>
@@ -2668,7 +2672,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -2679,7 +2683,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
+      <c r="A85" s="16"/>
       <c r="B85" s="1" t="s">
         <v>247</v>
       </c>
@@ -2965,7 +2969,7 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
+      <c r="A117" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B117" s="1" t="s">
@@ -2979,7 +2983,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A118" s="15"/>
+      <c r="A118" s="16"/>
       <c r="B118" s="1" t="s">
         <v>121</v>
       </c>
@@ -3232,7 +3236,9 @@
       <c r="A141" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B141" s="9"/>
+      <c r="B141" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C141" s="8" t="s">
         <v>308</v>
       </c>
@@ -3244,7 +3250,9 @@
       <c r="A142" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B142" s="9"/>
+      <c r="B142" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C142" s="8" t="s">
         <v>308</v>
       </c>
@@ -3257,7 +3265,9 @@
         <v>193</v>
       </c>
       <c r="B143" s="9"/>
-      <c r="C143" s="9"/>
+      <c r="C143" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="D143" s="8" t="s">
         <v>308</v>
       </c>
@@ -3428,7 +3438,7 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A163" s="14" t="s">
+      <c r="A163" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B163" s="1" t="s">
@@ -3442,7 +3452,7 @@
       </c>
     </row>
     <row r="164" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="16"/>
       <c r="B164" s="1" t="s">
         <v>150</v>
       </c>
@@ -3537,7 +3547,9 @@
       <c r="A171" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B171" s="9"/>
+      <c r="B171" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C171" s="8" t="s">
         <v>308</v>
       </c>
@@ -3699,7 +3711,7 @@
       </c>
     </row>
     <row r="188" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A188" s="14" t="s">
+      <c r="A188" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B188" s="1" t="s">
@@ -3716,7 +3728,7 @@
       </c>
     </row>
     <row r="189" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A189" s="15"/>
+      <c r="A189" s="16"/>
       <c r="B189" s="1" t="s">
         <v>157</v>
       </c>
@@ -3803,7 +3815,9 @@
       <c r="A195" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="B195" s="9"/>
+      <c r="B195" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C195" s="8" t="s">
         <v>308</v>
       </c>
@@ -3833,7 +3847,9 @@
       <c r="A197" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B197" s="9"/>
+      <c r="B197" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C197" s="8" t="s">
         <v>308</v>
       </c>
@@ -3861,7 +3877,9 @@
       <c r="A199" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B199" s="9"/>
+      <c r="B199" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C199" s="8" t="s">
         <v>308</v>
       </c>
@@ -3876,7 +3894,9 @@
       <c r="A200" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B200" s="9"/>
+      <c r="B200" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C200" s="8" t="s">
         <v>308</v>
       </c>
@@ -4111,7 +4131,7 @@
       </c>
     </row>
     <row r="222" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A222" s="14" t="s">
+      <c r="A222" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -4122,7 +4142,7 @@
       </c>
     </row>
     <row r="223" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A223" s="15"/>
+      <c r="A223" s="16"/>
       <c r="B223" s="1" t="s">
         <v>265</v>
       </c>
@@ -4458,7 +4478,7 @@
       </c>
     </row>
     <row r="261" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A261" s="14" t="s">
+      <c r="A261" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B261" s="1" t="s">
@@ -4475,7 +4495,7 @@
       </c>
     </row>
     <row r="262" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A262" s="15"/>
+      <c r="A262" s="16"/>
       <c r="B262" s="1" t="s">
         <v>175</v>
       </c>
@@ -4894,7 +4914,7 @@
       </c>
     </row>
     <row r="295" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A295" s="14" t="s">
+      <c r="A295" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B295" s="1" t="s">
@@ -4906,7 +4926,7 @@
       </c>
     </row>
     <row r="296" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A296" s="15"/>
+      <c r="A296" s="16"/>
       <c r="B296" s="1" t="s">
         <v>208</v>
       </c>
@@ -4922,7 +4942,7 @@
         <v>191</v>
       </c>
       <c r="B297" s="9"/>
-      <c r="C297" s="16" t="s">
+      <c r="C297" s="14" t="s">
         <v>294</v>
       </c>
       <c r="D297" s="7" t="s">
@@ -4936,7 +4956,7 @@
       <c r="B298" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C298" s="16"/>
+      <c r="C298" s="14"/>
       <c r="D298" s="7" t="s">
         <v>313</v>
       </c>
@@ -4948,7 +4968,7 @@
       <c r="B299" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C299" s="16"/>
+      <c r="C299" s="14"/>
       <c r="D299" s="7" t="s">
         <v>313</v>
       </c>
@@ -4960,7 +4980,7 @@
       <c r="B300" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C300" s="16"/>
+      <c r="C300" s="14"/>
       <c r="D300" s="7" t="s">
         <v>313</v>
       </c>
@@ -4972,7 +4992,7 @@
       <c r="B301" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C301" s="16"/>
+      <c r="C301" s="14"/>
       <c r="D301" s="8" t="s">
         <v>308</v>
       </c>
@@ -4984,7 +5004,7 @@
       <c r="B302" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="C302" s="16"/>
+      <c r="C302" s="14"/>
       <c r="D302" s="7" t="s">
         <v>313</v>
       </c>
@@ -4996,7 +5016,7 @@
       <c r="B303" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C303" s="16"/>
+      <c r="C303" s="14"/>
       <c r="D303" s="8" t="s">
         <v>308</v>
       </c>
@@ -5006,7 +5026,7 @@
         <v>55</v>
       </c>
       <c r="B304" s="9"/>
-      <c r="C304" s="16"/>
+      <c r="C304" s="14"/>
       <c r="D304" s="7" t="s">
         <v>313</v>
       </c>
@@ -5018,7 +5038,7 @@
       <c r="B305" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C305" s="16"/>
+      <c r="C305" s="14"/>
       <c r="D305" s="8" t="s">
         <v>308</v>
       </c>
@@ -5030,7 +5050,7 @@
       <c r="B306" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C306" s="16"/>
+      <c r="C306" s="14"/>
       <c r="D306" s="8" t="s">
         <v>308</v>
       </c>
@@ -5040,7 +5060,7 @@
         <v>193</v>
       </c>
       <c r="B307" s="9"/>
-      <c r="C307" s="16"/>
+      <c r="C307" s="14"/>
       <c r="D307" s="7" t="s">
         <v>313</v>
       </c>
@@ -5050,7 +5070,7 @@
         <v>56</v>
       </c>
       <c r="B308" s="9"/>
-      <c r="C308" s="16"/>
+      <c r="C308" s="14"/>
       <c r="D308" s="7" t="s">
         <v>313</v>
       </c>
@@ -5060,7 +5080,7 @@
         <v>11</v>
       </c>
       <c r="B309" s="9"/>
-      <c r="C309" s="16"/>
+      <c r="C309" s="14"/>
       <c r="D309" s="7" t="s">
         <v>313</v>
       </c>
@@ -5070,7 +5090,7 @@
         <v>1</v>
       </c>
       <c r="B310" s="9"/>
-      <c r="C310" s="16"/>
+      <c r="C310" s="14"/>
       <c r="D310" s="7" t="s">
         <v>313</v>
       </c>
@@ -5080,7 +5100,7 @@
         <v>211</v>
       </c>
       <c r="B311" s="9"/>
-      <c r="C311" s="16"/>
+      <c r="C311" s="14"/>
       <c r="D311" s="7" t="s">
         <v>313</v>
       </c>
@@ -5090,7 +5110,7 @@
         <v>57</v>
       </c>
       <c r="B312" s="9"/>
-      <c r="C312" s="16"/>
+      <c r="C312" s="14"/>
       <c r="D312" s="7" t="s">
         <v>313</v>
       </c>
@@ -5100,7 +5120,7 @@
         <v>63</v>
       </c>
       <c r="B313" s="9"/>
-      <c r="C313" s="16"/>
+      <c r="C313" s="14"/>
       <c r="D313" s="7" t="s">
         <v>313</v>
       </c>
@@ -5110,7 +5130,7 @@
         <v>206</v>
       </c>
       <c r="B314" s="9"/>
-      <c r="C314" s="16"/>
+      <c r="C314" s="14"/>
       <c r="D314" s="7" t="s">
         <v>313</v>
       </c>
@@ -5121,7 +5141,7 @@
       </c>
     </row>
     <row r="318" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A318" s="14" t="s">
+      <c r="A318" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B318" s="1" t="s">
@@ -5135,7 +5155,7 @@
       </c>
     </row>
     <row r="319" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A319" s="15"/>
+      <c r="A319" s="16"/>
       <c r="B319" s="1" t="s">
         <v>185</v>
       </c>
@@ -5536,7 +5556,7 @@
       </c>
     </row>
     <row r="355" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A355" s="14" t="s">
+      <c r="A355" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B355" s="1" t="s">
@@ -5553,7 +5573,7 @@
       </c>
     </row>
     <row r="356" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A356" s="15"/>
+      <c r="A356" s="16"/>
       <c r="B356" s="1" t="s">
         <v>79</v>
       </c>
@@ -6609,7 +6629,7 @@
       </c>
     </row>
     <row r="442" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A442" s="14" t="s">
+      <c r="A442" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B442" s="1" t="s">
@@ -6620,7 +6640,7 @@
       </c>
     </row>
     <row r="443" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A443" s="15"/>
+      <c r="A443" s="16"/>
       <c r="B443" s="1" t="s">
         <v>223</v>
       </c>
@@ -7063,6 +7083,13 @@
     <sortCondition ref="A9:A80"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="A318:A319"/>
+    <mergeCell ref="A355:A356"/>
+    <mergeCell ref="A442:A443"/>
+    <mergeCell ref="A188:A189"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="A261:A262"/>
+    <mergeCell ref="A295:A296"/>
     <mergeCell ref="C297:C314"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A84:A85"/>
@@ -7073,13 +7100,6 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="A117:A118"/>
     <mergeCell ref="A163:A164"/>
-    <mergeCell ref="A318:A319"/>
-    <mergeCell ref="A355:A356"/>
-    <mergeCell ref="A442:A443"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="A261:A262"/>
-    <mergeCell ref="A295:A296"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Interface Revisions Add missing "Introduced" test in several places, no change to dates.
</commit_message>
<xml_diff>
--- a/InstallerContent/ASCOMInterfaceRevisions.xlsx
+++ b/InstallerContent/ASCOMInterfaceRevisions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ASCOMPlatform\InstallerContent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5CAF4C-0C49-4DAA-A783-C369B071BB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24686642-6313-4973-9ECC-38DFED4A147A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C77C0BB1-9FCB-4A82-8AED-44FFC5395220}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="319">
   <si>
     <t>Telescope</t>
   </si>
@@ -1236,14 +1236,14 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1607,10 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCFDDAB-B80A-4B5D-BA40-62EFE29ED36B}">
   <dimension ref="A1:F493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A358" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A358" sqref="A358"/>
-      <selection pane="bottomLeft" activeCell="A361" sqref="A361"/>
+    <sheetView tabSelected="1" topLeftCell="A383" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1663,7 +1661,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1683,7 +1681,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1" t="s">
         <v>83</v>
       </c>
@@ -2758,7 +2756,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
+      <c r="A88" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2769,7 +2767,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
+      <c r="A89" s="16"/>
       <c r="B89" s="1" t="s">
         <v>247</v>
       </c>
@@ -3055,7 +3053,7 @@
       </c>
     </row>
     <row r="121" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="14" t="s">
+      <c r="A121" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B121" s="1" t="s">
@@ -3069,7 +3067,7 @@
       </c>
     </row>
     <row r="122" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A122" s="15"/>
+      <c r="A122" s="16"/>
       <c r="B122" s="1" t="s">
         <v>121</v>
       </c>
@@ -3300,7 +3298,9 @@
       <c r="A143" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="B143" s="9"/>
+      <c r="B143" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C143" s="8" t="s">
         <v>308</v>
       </c>
@@ -3524,7 +3524,7 @@
       </c>
     </row>
     <row r="167" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A167" s="14" t="s">
+      <c r="A167" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B167" s="1" t="s">
@@ -3538,7 +3538,7 @@
       </c>
     </row>
     <row r="168" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="16"/>
       <c r="B168" s="1" t="s">
         <v>150</v>
       </c>
@@ -3659,7 +3659,9 @@
       <c r="A177" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="B177" s="9"/>
+      <c r="B177" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C177" s="8" t="s">
         <v>308</v>
       </c>
@@ -3671,7 +3673,9 @@
       <c r="A178" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="B178" s="9"/>
+      <c r="B178" s="7" t="s">
+        <v>313</v>
+      </c>
       <c r="C178" s="8" t="s">
         <v>308</v>
       </c>
@@ -3797,7 +3801,7 @@
       </c>
     </row>
     <row r="192" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A192" s="14" t="s">
+      <c r="A192" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -3814,7 +3818,7 @@
       </c>
     </row>
     <row r="193" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A193" s="15"/>
+      <c r="A193" s="16"/>
       <c r="B193" s="1" t="s">
         <v>157</v>
       </c>
@@ -4217,7 +4221,7 @@
       </c>
     </row>
     <row r="226" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A226" s="14" t="s">
+      <c r="A226" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -4228,7 +4232,7 @@
       </c>
     </row>
     <row r="227" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A227" s="15"/>
+      <c r="A227" s="16"/>
       <c r="B227" s="1" t="s">
         <v>265</v>
       </c>
@@ -4564,7 +4568,7 @@
       </c>
     </row>
     <row r="265" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A265" s="14" t="s">
+      <c r="A265" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B265" s="1" t="s">
@@ -4581,7 +4585,7 @@
       </c>
     </row>
     <row r="266" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A266" s="15"/>
+      <c r="A266" s="16"/>
       <c r="B266" s="1" t="s">
         <v>175</v>
       </c>
@@ -5000,7 +5004,7 @@
       </c>
     </row>
     <row r="299" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A299" s="14" t="s">
+      <c r="A299" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B299" s="1" t="s">
@@ -5012,7 +5016,7 @@
       </c>
     </row>
     <row r="300" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A300" s="15"/>
+      <c r="A300" s="16"/>
       <c r="B300" s="1" t="s">
         <v>208</v>
       </c>
@@ -5028,7 +5032,7 @@
         <v>191</v>
       </c>
       <c r="B301" s="9"/>
-      <c r="C301" s="16" t="s">
+      <c r="C301" s="14" t="s">
         <v>294</v>
       </c>
       <c r="D301" s="7" t="s">
@@ -5042,7 +5046,7 @@
       <c r="B302" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C302" s="16"/>
+      <c r="C302" s="14"/>
       <c r="D302" s="7" t="s">
         <v>313</v>
       </c>
@@ -5054,7 +5058,7 @@
       <c r="B303" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C303" s="16"/>
+      <c r="C303" s="14"/>
       <c r="D303" s="7" t="s">
         <v>313</v>
       </c>
@@ -5066,7 +5070,7 @@
       <c r="B304" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C304" s="16"/>
+      <c r="C304" s="14"/>
       <c r="D304" s="7" t="s">
         <v>313</v>
       </c>
@@ -5078,7 +5082,7 @@
       <c r="B305" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C305" s="16"/>
+      <c r="C305" s="14"/>
       <c r="D305" s="8" t="s">
         <v>308</v>
       </c>
@@ -5090,7 +5094,7 @@
       <c r="B306" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="C306" s="16"/>
+      <c r="C306" s="14"/>
       <c r="D306" s="7" t="s">
         <v>313</v>
       </c>
@@ -5102,7 +5106,7 @@
       <c r="B307" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C307" s="16"/>
+      <c r="C307" s="14"/>
       <c r="D307" s="8" t="s">
         <v>308</v>
       </c>
@@ -5112,7 +5116,7 @@
         <v>55</v>
       </c>
       <c r="B308" s="9"/>
-      <c r="C308" s="16"/>
+      <c r="C308" s="14"/>
       <c r="D308" s="7" t="s">
         <v>313</v>
       </c>
@@ -5124,7 +5128,7 @@
       <c r="B309" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C309" s="16"/>
+      <c r="C309" s="14"/>
       <c r="D309" s="8" t="s">
         <v>308</v>
       </c>
@@ -5136,7 +5140,7 @@
       <c r="B310" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C310" s="16"/>
+      <c r="C310" s="14"/>
       <c r="D310" s="8" t="s">
         <v>308</v>
       </c>
@@ -5146,7 +5150,7 @@
         <v>193</v>
       </c>
       <c r="B311" s="9"/>
-      <c r="C311" s="16"/>
+      <c r="C311" s="14"/>
       <c r="D311" s="7" t="s">
         <v>313</v>
       </c>
@@ -5156,7 +5160,7 @@
         <v>56</v>
       </c>
       <c r="B312" s="9"/>
-      <c r="C312" s="16"/>
+      <c r="C312" s="14"/>
       <c r="D312" s="7" t="s">
         <v>313</v>
       </c>
@@ -5166,7 +5170,7 @@
         <v>11</v>
       </c>
       <c r="B313" s="9"/>
-      <c r="C313" s="16"/>
+      <c r="C313" s="14"/>
       <c r="D313" s="7" t="s">
         <v>313</v>
       </c>
@@ -5176,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="B314" s="9"/>
-      <c r="C314" s="16"/>
+      <c r="C314" s="14"/>
       <c r="D314" s="7" t="s">
         <v>313</v>
       </c>
@@ -5186,7 +5190,7 @@
         <v>211</v>
       </c>
       <c r="B315" s="9"/>
-      <c r="C315" s="16"/>
+      <c r="C315" s="14"/>
       <c r="D315" s="7" t="s">
         <v>313</v>
       </c>
@@ -5196,7 +5200,7 @@
         <v>57</v>
       </c>
       <c r="B316" s="9"/>
-      <c r="C316" s="16"/>
+      <c r="C316" s="14"/>
       <c r="D316" s="7" t="s">
         <v>313</v>
       </c>
@@ -5206,7 +5210,7 @@
         <v>63</v>
       </c>
       <c r="B317" s="9"/>
-      <c r="C317" s="16"/>
+      <c r="C317" s="14"/>
       <c r="D317" s="7" t="s">
         <v>313</v>
       </c>
@@ -5216,7 +5220,7 @@
         <v>206</v>
       </c>
       <c r="B318" s="9"/>
-      <c r="C318" s="16"/>
+      <c r="C318" s="14"/>
       <c r="D318" s="7" t="s">
         <v>313</v>
       </c>
@@ -5227,7 +5231,7 @@
       </c>
     </row>
     <row r="322" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A322" s="14" t="s">
+      <c r="A322" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B322" s="1" t="s">
@@ -5241,7 +5245,7 @@
       </c>
     </row>
     <row r="323" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A323" s="15"/>
+      <c r="A323" s="16"/>
       <c r="B323" s="1" t="s">
         <v>185</v>
       </c>
@@ -5642,7 +5646,7 @@
       </c>
     </row>
     <row r="359" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A359" s="14" t="s">
+      <c r="A359" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B359" s="1" t="s">
@@ -5659,7 +5663,7 @@
       </c>
     </row>
     <row r="360" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A360" s="15"/>
+      <c r="A360" s="16"/>
       <c r="B360" s="1" t="s">
         <v>79</v>
       </c>
@@ -6715,7 +6719,7 @@
       </c>
     </row>
     <row r="446" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A446" s="14" t="s">
+      <c r="A446" s="15" t="s">
         <v>292</v>
       </c>
       <c r="B446" s="1" t="s">
@@ -6726,7 +6730,7 @@
       </c>
     </row>
     <row r="447" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A447" s="15"/>
+      <c r="A447" s="16"/>
       <c r="B447" s="1" t="s">
         <v>223</v>
       </c>
@@ -7169,6 +7173,13 @@
     <sortCondition ref="A9:A84"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="A322:A323"/>
+    <mergeCell ref="A359:A360"/>
+    <mergeCell ref="A446:A447"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A226:A227"/>
+    <mergeCell ref="A265:A266"/>
+    <mergeCell ref="A299:A300"/>
     <mergeCell ref="C301:C318"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A88:A89"/>
@@ -7179,18 +7190,11 @@
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="A121:A122"/>
     <mergeCell ref="A167:A168"/>
-    <mergeCell ref="A322:A323"/>
-    <mergeCell ref="A359:A360"/>
-    <mergeCell ref="A446:A447"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="A226:A227"/>
-    <mergeCell ref="A265:A266"/>
-    <mergeCell ref="A299:A300"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;F &amp;D</oddFooter>
+    <oddFooter>&amp;L&amp;F &amp;D&amp;C&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="6" manualBreakCount="6">
     <brk id="86" max="16383" man="1"/>

</xml_diff>